<commit_message>
Changes for the revision
</commit_message>
<xml_diff>
--- a/Mobility_data/Other_input/Table_Dependent_Variables_basic.xlsx
+++ b/Mobility_data/Other_input/Table_Dependent_Variables_basic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
   <si>
     <t>varname</t>
   </si>
@@ -297,6 +297,15 @@
   </si>
   <si>
     <t>remove_na</t>
+  </si>
+  <si>
+    <t>Migration_background</t>
+  </si>
+  <si>
+    <t>P_MIG</t>
+  </si>
+  <si>
+    <t>1 is yes, 2 is no / 9: keine Angabe</t>
   </si>
 </sst>
 </file>
@@ -621,21 +630,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1"/>
-    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="43.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -661,7 +670,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -687,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -713,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -739,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -765,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -791,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -817,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -843,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -869,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -895,64 +904,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
       <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
         <v>43</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>11</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -973,12 +982,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -999,12 +1008,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
@@ -1016,7 +1025,7 @@
         <v>9</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1025,38 +1034,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="E16">
         <v>9</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -1077,12 +1086,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -1103,12 +1112,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -1120,30 +1129,30 @@
         <v>9</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1155,64 +1164,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
       <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
         <v>41</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>9</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22">
-        <v>7</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
-        <v>50</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
@@ -1233,12 +1242,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
         <v>40</v>
@@ -1259,64 +1268,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>89</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>57</v>
-      </c>
-      <c r="C25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>23</v>
       </c>
       <c r="C26" t="s">
         <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
@@ -1337,12 +1346,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
         <v>56</v>
@@ -1363,21 +1372,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>56</v>
       </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
       <c r="E29">
-        <v>1E+18</v>
+        <v>8</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1386,12 +1398,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
         <v>56</v>
@@ -1409,29 +1421,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
         <v>56</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31">
+        <v>1E+18</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" t="s">
         <v>80</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>8</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
         <v>0</v>
       </c>
     </row>

</xml_diff>